<commit_message>
Added intitial 4 layer board layout and made very minor changes to Schematic and BOM.
</commit_message>
<xml_diff>
--- a/Hardware/bom_r2.xlsx
+++ b/Hardware/bom_r2.xlsx
@@ -52,9 +52,6 @@
     <t>R1210</t>
   </si>
   <si>
-    <t>R10</t>
-  </si>
-  <si>
     <t>RESISTOR, American symbol</t>
   </si>
   <si>
@@ -557,6 +554,9 @@
   </si>
   <si>
     <t>JP2,</t>
+  </si>
+  <si>
+    <t>R10, R16</t>
   </si>
 </sst>
 </file>
@@ -1417,7 +1417,7 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1461,13 +1461,13 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1478,30 +1478,30 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
       </c>
       <c r="F2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G2" t="s">
         <v>84</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
+        <v>86</v>
+      </c>
+      <c r="J2" t="s">
         <v>85</v>
-      </c>
-      <c r="H2" t="s">
-        <v>87</v>
-      </c>
-      <c r="J2" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -1510,19 +1510,19 @@
         <v>11</v>
       </c>
       <c r="E3" t="s">
+        <v>180</v>
+      </c>
+      <c r="F3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
       <c r="G3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1530,28 +1530,28 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>16</v>
       </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
       <c r="F4" t="s">
+        <v>96</v>
+      </c>
+      <c r="G4" t="s">
         <v>97</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
+        <v>99</v>
+      </c>
+      <c r="J4" t="s">
         <v>98</v>
-      </c>
-      <c r="H4" t="s">
-        <v>100</v>
-      </c>
-      <c r="J4" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1559,28 +1559,28 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
         <v>18</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>19</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>20</v>
       </c>
-      <c r="E5" t="s">
-        <v>21</v>
-      </c>
       <c r="F5" t="s">
+        <v>96</v>
+      </c>
+      <c r="G5" t="s">
         <v>97</v>
       </c>
-      <c r="G5" t="s">
-        <v>98</v>
-      </c>
       <c r="H5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1588,28 +1588,28 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
         <v>22</v>
       </c>
-      <c r="D6" t="s">
-        <v>23</v>
-      </c>
       <c r="E6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F6" t="s">
+        <v>96</v>
+      </c>
+      <c r="G6" t="s">
         <v>97</v>
       </c>
-      <c r="G6" t="s">
-        <v>98</v>
-      </c>
       <c r="H6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1617,28 +1617,28 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
         <v>22</v>
       </c>
-      <c r="D7" t="s">
-        <v>23</v>
-      </c>
       <c r="E7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F7" t="s">
+        <v>96</v>
+      </c>
+      <c r="G7" t="s">
         <v>97</v>
       </c>
-      <c r="G7" t="s">
-        <v>98</v>
-      </c>
       <c r="H7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1646,28 +1646,28 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
         <v>24</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>25</v>
       </c>
-      <c r="E8" t="s">
-        <v>26</v>
-      </c>
       <c r="F8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1675,28 +1675,28 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
         <v>27</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>28</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>29</v>
       </c>
-      <c r="E9" t="s">
-        <v>30</v>
-      </c>
       <c r="F9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1704,28 +1704,28 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" t="s">
         <v>31</v>
       </c>
-      <c r="C10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" t="s">
-        <v>32</v>
-      </c>
       <c r="F10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1733,31 +1733,31 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
+        <v>176</v>
+      </c>
+      <c r="C11" t="s">
+        <v>171</v>
+      </c>
+      <c r="D11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" t="s">
+        <v>172</v>
+      </c>
+      <c r="F11" t="s">
+        <v>106</v>
+      </c>
+      <c r="G11" t="s">
+        <v>175</v>
+      </c>
+      <c r="H11" t="s">
         <v>177</v>
       </c>
-      <c r="C11" t="s">
-        <v>172</v>
-      </c>
-      <c r="D11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="I11" t="s">
+        <v>174</v>
+      </c>
+      <c r="J11" t="s">
         <v>173</v>
-      </c>
-      <c r="F11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G11" t="s">
-        <v>176</v>
-      </c>
-      <c r="H11" t="s">
-        <v>178</v>
-      </c>
-      <c r="I11" t="s">
-        <v>175</v>
-      </c>
-      <c r="J11" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1765,28 +1765,28 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" t="s">
         <v>33</v>
       </c>
-      <c r="C12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" t="s">
-        <v>34</v>
-      </c>
       <c r="F12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1794,28 +1794,28 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
         <v>35</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>36</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
+        <v>169</v>
+      </c>
+      <c r="F13" t="s">
         <v>37</v>
       </c>
-      <c r="E13" t="s">
-        <v>170</v>
-      </c>
-      <c r="F13" t="s">
-        <v>38</v>
-      </c>
       <c r="G13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H13" t="s">
+        <v>78</v>
+      </c>
+      <c r="J13" t="s">
         <v>79</v>
-      </c>
-      <c r="J13" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1823,28 +1823,28 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
         <v>39</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>40</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>41</v>
       </c>
-      <c r="E14" t="s">
-        <v>42</v>
-      </c>
       <c r="F14" t="s">
+        <v>96</v>
+      </c>
+      <c r="G14" t="s">
         <v>97</v>
       </c>
-      <c r="G14" t="s">
-        <v>98</v>
-      </c>
       <c r="H14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1852,28 +1852,28 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" t="s">
         <v>43</v>
       </c>
-      <c r="C15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" t="s">
-        <v>44</v>
-      </c>
       <c r="F15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1881,28 +1881,28 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" t="s">
         <v>45</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>46</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>47</v>
       </c>
-      <c r="E16" t="s">
-        <v>48</v>
-      </c>
       <c r="F16" t="s">
+        <v>127</v>
+      </c>
+      <c r="G16" t="s">
         <v>128</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
+        <v>130</v>
+      </c>
+      <c r="J16" t="s">
         <v>129</v>
-      </c>
-      <c r="H16" t="s">
-        <v>131</v>
-      </c>
-      <c r="J16" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1910,28 +1910,28 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" t="s">
         <v>49</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>50</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>51</v>
       </c>
-      <c r="E17" t="s">
-        <v>52</v>
-      </c>
       <c r="F17" t="s">
+        <v>131</v>
+      </c>
+      <c r="G17" t="s">
         <v>132</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
+        <v>134</v>
+      </c>
+      <c r="J17" t="s">
         <v>133</v>
-      </c>
-      <c r="H17" t="s">
-        <v>135</v>
-      </c>
-      <c r="J17" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1939,28 +1939,28 @@
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" t="s">
         <v>24</v>
       </c>
-      <c r="D18" t="s">
-        <v>25</v>
-      </c>
       <c r="E18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1968,28 +1968,28 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" t="s">
         <v>54</v>
       </c>
-      <c r="C19" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" t="s">
-        <v>41</v>
-      </c>
-      <c r="E19" t="s">
-        <v>55</v>
-      </c>
       <c r="F19" t="s">
+        <v>96</v>
+      </c>
+      <c r="G19" t="s">
         <v>97</v>
       </c>
-      <c r="G19" t="s">
-        <v>98</v>
-      </c>
       <c r="H19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1997,28 +1997,28 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" t="s">
         <v>15</v>
       </c>
-      <c r="D20" t="s">
-        <v>16</v>
-      </c>
       <c r="E20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F20" t="s">
+        <v>96</v>
+      </c>
+      <c r="G20" t="s">
         <v>97</v>
       </c>
-      <c r="G20" t="s">
-        <v>98</v>
-      </c>
       <c r="H20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -2026,28 +2026,28 @@
         <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" t="s">
         <v>24</v>
       </c>
-      <c r="D21" t="s">
-        <v>25</v>
-      </c>
       <c r="E21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J21" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -2055,25 +2055,25 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" t="s">
+        <v>140</v>
+      </c>
+      <c r="D22" t="s">
         <v>58</v>
       </c>
-      <c r="C22" t="s">
-        <v>141</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>59</v>
       </c>
-      <c r="E22" t="s">
-        <v>60</v>
-      </c>
       <c r="G22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H22" t="s">
+        <v>142</v>
+      </c>
+      <c r="I22" t="s">
         <v>143</v>
-      </c>
-      <c r="I22" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -2081,28 +2081,28 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" t="s">
+        <v>139</v>
+      </c>
+      <c r="D23" t="s">
+        <v>136</v>
+      </c>
+      <c r="E23" t="s">
         <v>61</v>
       </c>
-      <c r="C23" t="s">
-        <v>140</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="G23" t="s">
+        <v>135</v>
+      </c>
+      <c r="H23" t="s">
+        <v>136</v>
+      </c>
+      <c r="I23" t="s">
+        <v>144</v>
+      </c>
+      <c r="J23" t="s">
         <v>137</v>
-      </c>
-      <c r="E23" t="s">
-        <v>62</v>
-      </c>
-      <c r="G23" t="s">
-        <v>136</v>
-      </c>
-      <c r="H23" t="s">
-        <v>137</v>
-      </c>
-      <c r="I23" t="s">
-        <v>145</v>
-      </c>
-      <c r="J23" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -2110,31 +2110,31 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" t="s">
         <v>63</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>64</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>65</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>66</v>
       </c>
-      <c r="F24" t="s">
-        <v>67</v>
-      </c>
       <c r="G24" t="s">
+        <v>145</v>
+      </c>
+      <c r="H24" t="s">
+        <v>148</v>
+      </c>
+      <c r="I24" t="s">
         <v>146</v>
       </c>
-      <c r="H24" t="s">
-        <v>149</v>
-      </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>147</v>
-      </c>
-      <c r="J24" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -2142,28 +2142,28 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" t="s">
+        <v>67</v>
+      </c>
+      <c r="D25" t="s">
         <v>68</v>
       </c>
-      <c r="C25" t="s">
-        <v>68</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>69</v>
       </c>
-      <c r="E25" t="s">
-        <v>70</v>
-      </c>
       <c r="F25" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G25" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I25" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -2171,31 +2171,31 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" t="s">
+        <v>70</v>
+      </c>
+      <c r="D26" t="s">
         <v>71</v>
       </c>
-      <c r="C26" t="s">
-        <v>71</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>72</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>73</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
+        <v>151</v>
+      </c>
+      <c r="H26" t="s">
+        <v>70</v>
+      </c>
+      <c r="I26" t="s">
+        <v>154</v>
+      </c>
+      <c r="J26" t="s">
         <v>74</v>
-      </c>
-      <c r="G26" t="s">
-        <v>152</v>
-      </c>
-      <c r="H26" t="s">
-        <v>71</v>
-      </c>
-      <c r="I26" t="s">
-        <v>155</v>
-      </c>
-      <c r="J26" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -2203,28 +2203,28 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
+        <v>161</v>
+      </c>
+      <c r="C27" t="s">
         <v>162</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>163</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>164</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>165</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>166</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>167</v>
       </c>
-      <c r="H27" t="s">
+      <c r="I27" t="s">
         <v>168</v>
-      </c>
-      <c r="I27" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -2232,36 +2232,36 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
+        <v>75</v>
+      </c>
+      <c r="C28" t="s">
+        <v>75</v>
+      </c>
+      <c r="D28" t="s">
+        <v>75</v>
+      </c>
+      <c r="E28" t="s">
+        <v>179</v>
+      </c>
+      <c r="F28" t="s">
         <v>76</v>
       </c>
-      <c r="C28" t="s">
-        <v>76</v>
-      </c>
-      <c r="D28" t="s">
-        <v>76</v>
-      </c>
-      <c r="E28" t="s">
-        <v>180</v>
-      </c>
-      <c r="F28" t="s">
-        <v>77</v>
-      </c>
       <c r="G28" t="s">
+        <v>158</v>
+      </c>
+      <c r="H28" t="s">
         <v>159</v>
       </c>
-      <c r="H28" t="s">
-        <v>160</v>
-      </c>
       <c r="J28" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated board and schematic as per recommendations.
</commit_message>
<xml_diff>
--- a/Hardware/bom_r2.xlsx
+++ b/Hardware/bom_r2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="182">
   <si>
     <t>Qty</t>
   </si>
@@ -520,9 +520,6 @@
     <t>MAX4995A</t>
   </si>
   <si>
-    <t>MAX4995AAUT+T-ND</t>
-  </si>
-  <si>
     <t>C26</t>
   </si>
   <si>
@@ -557,6 +554,12 @@
   </si>
   <si>
     <t>R10, R16</t>
+  </si>
+  <si>
+    <t>Mouser Part Number</t>
+  </si>
+  <si>
+    <t>700-MAX4995AAUTT</t>
   </si>
 </sst>
 </file>
@@ -1107,9 +1110,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K28" totalsRowShown="0">
-  <autoFilter ref="A1:K28"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L28" totalsRowShown="0">
+  <autoFilter ref="A1:L28"/>
+  <tableColumns count="12">
     <tableColumn id="1" name="Qty"/>
     <tableColumn id="2" name="Value"/>
     <tableColumn id="3" name="Device"/>
@@ -1119,6 +1122,7 @@
     <tableColumn id="7" name="MF"/>
     <tableColumn id="8" name="MPN"/>
     <tableColumn id="9" name="Digikey Part Number"/>
+    <tableColumn id="11" name="Mouser Part Number"/>
     <tableColumn id="10" name="Newark Part Number"/>
     <tableColumn id="12" name="Sparkfun Part Number"/>
   </tableColumns>
@@ -1414,10 +1418,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1435,7 +1439,7 @@
     <col min="11" max="11" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1464,13 +1468,16 @@
         <v>141</v>
       </c>
       <c r="J1" t="s">
+        <v>180</v>
+      </c>
+      <c r="K1" t="s">
         <v>77</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1492,11 +1499,11 @@
       <c r="H2" t="s">
         <v>86</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1510,7 +1517,7 @@
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
@@ -1521,11 +1528,11 @@
       <c r="H3" t="s">
         <v>88</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1550,11 +1557,11 @@
       <c r="H4" t="s">
         <v>99</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1579,11 +1586,11 @@
       <c r="H5" t="s">
         <v>101</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>15</v>
       </c>
@@ -1597,7 +1604,7 @@
         <v>22</v>
       </c>
       <c r="E6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F6" t="s">
         <v>96</v>
@@ -1608,11 +1615,11 @@
       <c r="H6" t="s">
         <v>103</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -1626,7 +1633,7 @@
         <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F7" t="s">
         <v>96</v>
@@ -1637,11 +1644,11 @@
       <c r="H7" t="s">
         <v>105</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1666,11 +1673,11 @@
       <c r="H8" t="s">
         <v>114</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1695,11 +1702,11 @@
       <c r="H9" t="s">
         <v>117</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1724,43 +1731,43 @@
       <c r="H10" t="s">
         <v>119</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D11" t="s">
         <v>28</v>
       </c>
       <c r="E11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F11" t="s">
         <v>106</v>
       </c>
       <c r="G11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I11" t="s">
-        <v>174</v>
-      </c>
-      <c r="J11" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K11" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1785,11 +1792,11 @@
       <c r="H12" t="s">
         <v>121</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1803,7 +1810,7 @@
         <v>36</v>
       </c>
       <c r="E13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F13" t="s">
         <v>37</v>
@@ -1814,11 +1821,11 @@
       <c r="H13" t="s">
         <v>78</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>4</v>
       </c>
@@ -1843,11 +1850,11 @@
       <c r="H14" t="s">
         <v>108</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1872,11 +1879,11 @@
       <c r="H15" t="s">
         <v>123</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
@@ -1901,11 +1908,11 @@
       <c r="H16" t="s">
         <v>130</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1930,11 +1937,11 @@
       <c r="H17" t="s">
         <v>134</v>
       </c>
-      <c r="J17" t="s">
+      <c r="K17" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>3</v>
       </c>
@@ -1959,11 +1966,11 @@
       <c r="H18" t="s">
         <v>124</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1988,11 +1995,11 @@
       <c r="H19" t="s">
         <v>110</v>
       </c>
-      <c r="J19" t="s">
+      <c r="K19" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1</v>
       </c>
@@ -2017,11 +2024,11 @@
       <c r="H20" t="s">
         <v>112</v>
       </c>
-      <c r="J20" t="s">
+      <c r="K20" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>4</v>
       </c>
@@ -2046,11 +2053,11 @@
       <c r="H21" t="s">
         <v>126</v>
       </c>
-      <c r="J21" t="s">
+      <c r="K21" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1</v>
       </c>
@@ -2076,7 +2083,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
@@ -2101,11 +2108,11 @@
       <c r="I23" t="s">
         <v>144</v>
       </c>
-      <c r="J23" t="s">
+      <c r="K23" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
@@ -2133,11 +2140,11 @@
       <c r="I24" t="s">
         <v>146</v>
       </c>
-      <c r="J24" t="s">
+      <c r="K24" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1</v>
       </c>
@@ -2166,7 +2173,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1</v>
       </c>
@@ -2194,11 +2201,11 @@
       <c r="I26" t="s">
         <v>154</v>
       </c>
-      <c r="J26" t="s">
+      <c r="K26" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1</v>
       </c>
@@ -2223,11 +2230,11 @@
       <c r="H27" t="s">
         <v>167</v>
       </c>
-      <c r="I27" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J27" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1</v>
       </c>
@@ -2241,7 +2248,7 @@
         <v>75</v>
       </c>
       <c r="E28" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F28" t="s">
         <v>76</v>
@@ -2252,14 +2259,14 @@
       <c r="H28" t="s">
         <v>159</v>
       </c>
-      <c r="J28" t="s">
+      <c r="K28" t="s">
         <v>157</v>
       </c>
-      <c r="K28" s="1" t="s">
+      <c r="L28" s="1" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>160</v>
       </c>

</xml_diff>

<commit_message>
Updated BOM to reflect layout changes.
</commit_message>
<xml_diff>
--- a/Hardware/bom_r2.xlsx
+++ b/Hardware/bom_r2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="175">
   <si>
     <t>Qty</t>
   </si>
@@ -40,12 +40,6 @@
     <t>MPN</t>
   </si>
   <si>
-    <t>JP2Q</t>
-  </si>
-  <si>
-    <t>JP1</t>
-  </si>
-  <si>
     <t>R-US_R1210</t>
   </si>
   <si>
@@ -265,18 +259,6 @@
     <t>Multicomp</t>
   </si>
   <si>
-    <t>Jumper/Header</t>
-  </si>
-  <si>
-    <t>Multicomp/FCI</t>
-  </si>
-  <si>
-    <t>84K8569(jumper) 33M7872 (Header )</t>
-  </si>
-  <si>
-    <t>SPC19807(jumper) 167997-204HLF(Header)</t>
-  </si>
-  <si>
     <t>72M6870</t>
   </si>
   <si>
@@ -362,9 +344,6 @@
   </si>
   <si>
     <t>8K4450</t>
-  </si>
-  <si>
-    <t>2x2, 2.54mm pin spacing</t>
   </si>
   <si>
     <t>MC0063W0603110K</t>
@@ -1110,8 +1089,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L28" totalsRowShown="0">
-  <autoFilter ref="A1:L28"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L27" totalsRowShown="0">
+  <autoFilter ref="A1:L27"/>
   <tableColumns count="12">
     <tableColumn id="1" name="Qty"/>
     <tableColumn id="2" name="Value"/>
@@ -1418,10 +1397,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1465,71 +1444,74 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="J1" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="K1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="L1" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>89</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>116</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>172</v>
       </c>
       <c r="F2" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="K2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>179</v>
+        <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>90</v>
       </c>
       <c r="G3" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="H3" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="K3" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1537,94 +1519,94 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="G4" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="H4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="K4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>170</v>
       </c>
       <c r="F5" t="s">
+        <v>90</v>
+      </c>
+      <c r="G5" t="s">
+        <v>91</v>
+      </c>
+      <c r="H5" t="s">
+        <v>97</v>
+      </c>
+      <c r="K5" t="s">
         <v>96</v>
-      </c>
-      <c r="G5" t="s">
-        <v>97</v>
-      </c>
-      <c r="H5" t="s">
-        <v>101</v>
-      </c>
-      <c r="K5" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="F6" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="G6" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="H6" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="K6" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C7" t="s">
         <v>21</v>
@@ -1633,77 +1615,77 @@
         <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>169</v>
+        <v>23</v>
       </c>
       <c r="F7" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="G7" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="H7" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="K7" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>91</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F8" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="K8" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
         <v>26</v>
-      </c>
-      <c r="C9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" t="s">
-        <v>28</v>
       </c>
       <c r="E9" t="s">
         <v>29</v>
       </c>
       <c r="F9" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H9" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="K9" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1711,28 +1693,31 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>168</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>163</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E10" t="s">
-        <v>31</v>
+        <v>164</v>
       </c>
       <c r="F10" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G10" t="s">
-        <v>82</v>
+        <v>167</v>
       </c>
       <c r="H10" t="s">
-        <v>119</v>
+        <v>169</v>
+      </c>
+      <c r="I10" t="s">
+        <v>166</v>
       </c>
       <c r="K10" t="s">
-        <v>118</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1740,31 +1725,28 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>175</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>170</v>
+        <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E11" t="s">
-        <v>171</v>
+        <v>31</v>
       </c>
       <c r="F11" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G11" t="s">
-        <v>174</v>
+        <v>80</v>
       </c>
       <c r="H11" t="s">
-        <v>176</v>
-      </c>
-      <c r="I11" t="s">
-        <v>173</v>
+        <v>114</v>
       </c>
       <c r="K11" t="s">
-        <v>172</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1775,106 +1757,106 @@
         <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E12" t="s">
-        <v>33</v>
+        <v>161</v>
       </c>
       <c r="F12" t="s">
-        <v>106</v>
+        <v>35</v>
       </c>
       <c r="G12" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="H12" t="s">
-        <v>121</v>
+        <v>76</v>
       </c>
       <c r="K12" t="s">
-        <v>120</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D13" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E13" t="s">
-        <v>168</v>
+        <v>39</v>
       </c>
       <c r="F13" t="s">
-        <v>37</v>
+        <v>90</v>
       </c>
       <c r="G13" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="H13" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="K13" t="s">
-        <v>79</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="D14" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="E14" t="s">
         <v>41</v>
       </c>
       <c r="F14" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="G14" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="H14" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="K14" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B15" t="s">
         <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="D15" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="E15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F15" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
       <c r="G15" t="s">
-        <v>82</v>
+        <v>121</v>
       </c>
       <c r="H15" t="s">
         <v>123</v>
@@ -1885,176 +1867,173 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D16" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E16" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F16" t="s">
+        <v>124</v>
+      </c>
+      <c r="G16" t="s">
+        <v>125</v>
+      </c>
+      <c r="H16" t="s">
         <v>127</v>
       </c>
-      <c r="G16" t="s">
-        <v>128</v>
-      </c>
-      <c r="H16" t="s">
-        <v>130</v>
-      </c>
       <c r="K16" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>86</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="D17" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" t="s">
         <v>50</v>
       </c>
-      <c r="E17" t="s">
-        <v>51</v>
-      </c>
       <c r="F17" t="s">
+        <v>100</v>
+      </c>
+      <c r="G17" t="s">
+        <v>80</v>
+      </c>
+      <c r="H17" t="s">
+        <v>117</v>
+      </c>
+      <c r="K17" t="s">
         <v>131</v>
-      </c>
-      <c r="G17" t="s">
-        <v>132</v>
-      </c>
-      <c r="H17" t="s">
-        <v>134</v>
-      </c>
-      <c r="K17" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>92</v>
+        <v>51</v>
       </c>
       <c r="C18" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="D18" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="E18" t="s">
         <v>52</v>
       </c>
       <c r="F18" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="G18" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="H18" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="K18" t="s">
-        <v>138</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B19" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" t="s">
         <v>53</v>
       </c>
-      <c r="C19" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" t="s">
-        <v>40</v>
-      </c>
-      <c r="E19" t="s">
-        <v>54</v>
-      </c>
       <c r="F19" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="G19" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="H19" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="K19" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C20" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D20" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F20" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="G20" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="H20" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="K20" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>94</v>
+        <v>55</v>
       </c>
       <c r="C21" t="s">
-        <v>23</v>
+        <v>133</v>
       </c>
       <c r="D21" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="E21" t="s">
-        <v>56</v>
-      </c>
-      <c r="F21" t="s">
-        <v>106</v>
+        <v>57</v>
       </c>
       <c r="G21" t="s">
-        <v>82</v>
+        <v>128</v>
       </c>
       <c r="H21" t="s">
-        <v>126</v>
-      </c>
-      <c r="K21" t="s">
-        <v>125</v>
+        <v>135</v>
+      </c>
+      <c r="I21" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -2062,25 +2041,28 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C22" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="D22" t="s">
-        <v>58</v>
+        <v>129</v>
       </c>
       <c r="E22" t="s">
         <v>59</v>
       </c>
       <c r="G22" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="H22" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="I22" t="s">
-        <v>143</v>
+        <v>137</v>
+      </c>
+      <c r="K22" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -2091,25 +2073,28 @@
         <v>60</v>
       </c>
       <c r="C23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" t="s">
+        <v>62</v>
+      </c>
+      <c r="E23" t="s">
+        <v>63</v>
+      </c>
+      <c r="F23" t="s">
+        <v>64</v>
+      </c>
+      <c r="G23" t="s">
+        <v>138</v>
+      </c>
+      <c r="H23" t="s">
+        <v>141</v>
+      </c>
+      <c r="I23" t="s">
         <v>139</v>
       </c>
-      <c r="D23" t="s">
-        <v>136</v>
-      </c>
-      <c r="E23" t="s">
-        <v>61</v>
-      </c>
-      <c r="G23" t="s">
-        <v>135</v>
-      </c>
-      <c r="H23" t="s">
-        <v>136</v>
-      </c>
-      <c r="I23" t="s">
-        <v>144</v>
-      </c>
       <c r="K23" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -2117,31 +2102,28 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C24" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D24" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E24" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F24" t="s">
-        <v>66</v>
+        <v>146</v>
       </c>
       <c r="G24" t="s">
         <v>145</v>
       </c>
       <c r="H24" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="I24" t="s">
-        <v>146</v>
-      </c>
-      <c r="K24" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -2149,28 +2131,31 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C25" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D25" t="s">
+        <v>69</v>
+      </c>
+      <c r="E25" t="s">
+        <v>70</v>
+      </c>
+      <c r="F25" t="s">
+        <v>71</v>
+      </c>
+      <c r="G25" t="s">
+        <v>144</v>
+      </c>
+      <c r="H25" t="s">
         <v>68</v>
       </c>
-      <c r="E25" t="s">
-        <v>69</v>
-      </c>
-      <c r="F25" t="s">
-        <v>153</v>
-      </c>
-      <c r="G25" t="s">
-        <v>152</v>
-      </c>
-      <c r="H25" t="s">
-        <v>150</v>
-      </c>
       <c r="I25" t="s">
-        <v>149</v>
+        <v>147</v>
+      </c>
+      <c r="K25" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -2178,31 +2163,28 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>70</v>
+        <v>154</v>
       </c>
       <c r="C26" t="s">
-        <v>70</v>
+        <v>155</v>
       </c>
       <c r="D26" t="s">
-        <v>71</v>
+        <v>156</v>
       </c>
       <c r="E26" t="s">
-        <v>72</v>
+        <v>157</v>
       </c>
       <c r="F26" t="s">
-        <v>73</v>
+        <v>158</v>
       </c>
       <c r="G26" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="H26" t="s">
-        <v>70</v>
-      </c>
-      <c r="I26" t="s">
-        <v>154</v>
-      </c>
-      <c r="K26" t="s">
-        <v>74</v>
+        <v>160</v>
+      </c>
+      <c r="J26" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -2210,65 +2192,36 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>161</v>
+        <v>73</v>
       </c>
       <c r="C27" t="s">
-        <v>162</v>
+        <v>73</v>
       </c>
       <c r="D27" t="s">
-        <v>163</v>
+        <v>73</v>
       </c>
       <c r="E27" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="F27" t="s">
-        <v>165</v>
+        <v>74</v>
       </c>
       <c r="G27" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="H27" t="s">
-        <v>167</v>
-      </c>
-      <c r="J27" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>1</v>
-      </c>
-      <c r="B28" t="s">
-        <v>75</v>
-      </c>
-      <c r="C28" t="s">
-        <v>75</v>
-      </c>
-      <c r="D28" t="s">
-        <v>75</v>
-      </c>
-      <c r="E28" t="s">
-        <v>178</v>
-      </c>
-      <c r="F28" t="s">
-        <v>76</v>
-      </c>
-      <c r="G28" t="s">
-        <v>158</v>
-      </c>
-      <c r="H28" t="s">
-        <v>159</v>
-      </c>
-      <c r="K28" t="s">
-        <v>157</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>160</v>
+        <v>152</v>
+      </c>
+      <c r="K27" t="s">
+        <v>150</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated BOM with qty and urls
</commit_message>
<xml_diff>
--- a/Hardware/bom_r2.xlsx
+++ b/Hardware/bom_r2.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="202">
   <si>
     <t>Qty</t>
   </si>
@@ -343,12 +343,6 @@
     <t>MC00625W0402110R</t>
   </si>
   <si>
-    <t>8K4450</t>
-  </si>
-  <si>
-    <t>MC0063W0603110K</t>
-  </si>
-  <si>
     <t>94W4696</t>
   </si>
   <si>
@@ -460,12 +454,6 @@
     <t>638-1086-ND</t>
   </si>
   <si>
-    <t>Sparkfun Part Number</t>
-  </si>
-  <si>
-    <t>PRT-09011</t>
-  </si>
-  <si>
     <t>31M6798</t>
   </si>
   <si>
@@ -475,9 +463,6 @@
     <t>87583-2010BLF</t>
   </si>
   <si>
-    <t>Goes with Board R.2 6/3/2015</t>
-  </si>
-  <si>
     <t>MAX4495AAUT</t>
   </si>
   <si>
@@ -539,13 +524,109 @@
   </si>
   <si>
     <t>700-MAX4995AAUTT</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Price ea.</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/vishay-dale/crcw12100000z0ea/resistor-chip-jumper-zero-ohm/dp/72M6870?ost=72M6870</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/avx/06035c103kat2a/ceramic-capacitor-0-01uf-50v-x7r/dp/36K3729?ost=36K3729</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/avx/08055c223kat2a/ceramic-capacitor-0-022uf-50v/dp/35K2132?ost=35K2132</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/avx/0402zd104kat2a/ceramic-capacitor-0-1uf-10v-x5r/dp/96M1117?ost=96M1117</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/avx/0402zd105kat2a/ceramic-capacitor-1uf-10v-x5r/dp/06M4041?ost=06M4041</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/multicomp/mc00625w0402110r/resistor-10r-0-063w-1-0402/dp/58K4201?ost=58K4201</t>
+  </si>
+  <si>
+    <t>86T3506</t>
+  </si>
+  <si>
+    <t>MCMR06X1002FTL</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/multicomp/mcmr06x1002ftl/resistor-ceramic-10k-0-1w-1/dp/86T3506</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/multicomp/mc0063w0603112k4/resistor-12k4-0-063w-1-0603/dp/94W4696?ost=94W4696</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?x=0&amp;y=0&amp;lang=en&amp;site=us&amp;keywords=1276-4545-1-ND</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/multicomp/mc0603saf1202t5e/thick-film-resistor-12kohm-100mw/dp/79M5909?ost=79M5909</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/panasonic-electronic-components/eeh-zc1v151p/aluminum-electrolytic-capacitor/dp/91T4915?ost=91T4915</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/avx/04025a150jat2a/ceramic-capacitor-15pf-50v-c0g/dp/96M1134?ost=96M1134</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/multicomp/mc00625w040211m/resistor-1m-0-063w-1-0402/dp/58K4211?ost=58K4211</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/murata/blm18pg121sn1d/ferrite-bead-120-ohm-2a-0603/dp/73M9109?ost=73M9109</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/abracon/abm3b-25-000mhz-b2-t/crystal-25mhz-18pf-5-x-3-2mm/dp/13J1745?ost=13J1745</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/multicomp/mc00625w04021330r/resistor-330r-0-063w-1-0402/dp/58K4323?ost=58K4323</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/avx/04025a330jat2a/ceramic-capacitor-33pf-50v-c0g/dp/96M1150?ost=96M1150</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/avx/06036d475kat2a/ceramic-capacitor-4-7uf-6-3v-x5r/dp/96M1295?ost=96M1295</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/multicomp/mc0402wgf499jtce/thick-film-resistor-49-9-ohm-63mw/dp/79M5889?ost=79M5889</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?KeyWords=H11630CT-ND&amp;WT.z_header=search_go</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?KeyWords=H11908CT-ND&amp;WT.z_header=search_go</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/lumex/sml-lx0805sgc-tr/led-green-1-25mm-x-1-4mm-15mcd/dp/09J9138?ost=09J9138</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?KeyWords=553-1350-ND&amp;WT.z_header=search_go</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/microchip/lan9512-jzx/usb-hub-ethernet-controller-100mbps/dp/69W9521?ost=66W1988&amp;rpsku=66W1988</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Maxim-Integrated/MAX4995AAUT+T/?qs=%2fha2pyFaduhSMe2qdQb6iOxZF3Hc4rE6tANG4LQrENv6a72d3RT0UA%3d%3d</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/fci/87583-2010blf/usb-2-0-type-a-recetpacle-smt/dp/31M6798?ost=31M6798</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price Ea. Order: </t>
+  </si>
+  <si>
+    <t>Price ea. Order</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -687,6 +768,20 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF333333"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -985,7 +1080,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1028,13 +1123,17 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" xfId="10"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1068,6 +1167,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1089,9 +1189,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L27" totalsRowShown="0">
-  <autoFilter ref="A1:L27"/>
-  <tableColumns count="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="BOM" displayName="BOM" ref="A1:N27" totalsRowShown="0">
+  <autoFilter ref="A1:N27"/>
+  <tableColumns count="14">
     <tableColumn id="1" name="Qty"/>
     <tableColumn id="2" name="Value"/>
     <tableColumn id="3" name="Device"/>
@@ -1103,7 +1203,11 @@
     <tableColumn id="9" name="Digikey Part Number"/>
     <tableColumn id="11" name="Mouser Part Number"/>
     <tableColumn id="10" name="Newark Part Number"/>
-    <tableColumn id="12" name="Sparkfun Part Number"/>
+    <tableColumn id="13" name="URL"/>
+    <tableColumn id="15" name="Price ea." dataCellStyle="Hyperlink"/>
+    <tableColumn id="12" name="Price ea. Order">
+      <calculatedColumnFormula>BOM[[#This Row],[Price ea.]]*BOM[[#This Row],[Qty]]</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1397,10 +1501,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1410,15 +1514,17 @@
     <col min="3" max="3" width="17.140625" customWidth="1"/>
     <col min="4" max="4" width="28.85546875" customWidth="1"/>
     <col min="5" max="5" width="29.140625" customWidth="1"/>
-    <col min="6" max="6" width="8" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" customWidth="1"/>
     <col min="8" max="8" width="24.85546875" customWidth="1"/>
     <col min="9" max="9" width="23.85546875" customWidth="1"/>
     <col min="10" max="10" width="21.140625" customWidth="1"/>
-    <col min="11" max="11" width="17.5703125" customWidth="1"/>
+    <col min="11" max="11" width="27.5703125" customWidth="1"/>
+    <col min="12" max="13" width="17.5703125" customWidth="1"/>
+    <col min="14" max="15" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1444,19 +1550,25 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="J1" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="K1" t="s">
         <v>75</v>
       </c>
       <c r="L1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+      <c r="M1" t="s">
+        <v>171</v>
+      </c>
+      <c r="N1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -1470,7 +1582,7 @@
         <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -1484,8 +1596,18 @@
       <c r="K2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L2" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="M2">
+        <v>0.248</v>
+      </c>
+      <c r="N2">
+        <f>BOM[[#This Row],[Price ea.]]*BOM[[#This Row],[Qty]]</f>
+        <v>0.496</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1513,8 +1635,18 @@
       <c r="K3" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L3" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="M3">
+        <v>2E-3</v>
+      </c>
+      <c r="N3">
+        <f>BOM[[#This Row],[Price ea.]]*BOM[[#This Row],[Qty]]</f>
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1542,8 +1674,18 @@
       <c r="K4" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L4" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="M4">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="N4">
+        <f>BOM[[#This Row],[Price ea.]]*BOM[[#This Row],[Qty]]</f>
+        <v>0.16200000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>15</v>
       </c>
@@ -1557,7 +1699,7 @@
         <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="F5" t="s">
         <v>90</v>
@@ -1571,8 +1713,18 @@
       <c r="K5" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L5" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="M5">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="N5">
+        <f>BOM[[#This Row],[Price ea.]]*BOM[[#This Row],[Qty]]</f>
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1586,7 +1738,7 @@
         <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="F6" t="s">
         <v>90</v>
@@ -1600,8 +1752,18 @@
       <c r="K6" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L6" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="M6">
+        <v>0.24</v>
+      </c>
+      <c r="N6">
+        <f>BOM[[#This Row],[Price ea.]]*BOM[[#This Row],[Qty]]</f>
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1629,8 +1791,18 @@
       <c r="K7" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L7" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="M7">
+        <v>2E-3</v>
+      </c>
+      <c r="N7">
+        <f>BOM[[#This Row],[Price ea.]]*BOM[[#This Row],[Qty]]</f>
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1652,14 +1824,24 @@
       <c r="G8" t="s">
         <v>80</v>
       </c>
-      <c r="H8" t="s">
-        <v>110</v>
-      </c>
-      <c r="K8" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H8" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="M8">
+        <v>1.6E-2</v>
+      </c>
+      <c r="N8">
+        <f>BOM[[#This Row],[Price ea.]]*BOM[[#This Row],[Qty]]</f>
+        <v>3.2000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1682,45 +1864,65 @@
         <v>80</v>
       </c>
       <c r="H9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K9" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="M9">
+        <v>1E-3</v>
+      </c>
+      <c r="N9">
+        <f>BOM[[#This Row],[Price ea.]]*BOM[[#This Row],[Qty]]</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C10" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D10" t="s">
         <v>26</v>
       </c>
       <c r="E10" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="F10" t="s">
         <v>100</v>
       </c>
       <c r="G10" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="H10" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="I10" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="K10" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="M10">
+        <v>0.1</v>
+      </c>
+      <c r="N10">
+        <f>BOM[[#This Row],[Price ea.]]*BOM[[#This Row],[Qty]]</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1743,13 +1945,23 @@
         <v>80</v>
       </c>
       <c r="H11" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K11" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="M11">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="N11">
+        <f>BOM[[#This Row],[Price ea.]]*BOM[[#This Row],[Qty]]</f>
+        <v>6.7000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1763,7 +1975,7 @@
         <v>34</v>
       </c>
       <c r="E12" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="F12" t="s">
         <v>35</v>
@@ -1777,8 +1989,18 @@
       <c r="K12" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L12" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="M12">
+        <v>3.39</v>
+      </c>
+      <c r="N12">
+        <f>BOM[[#This Row],[Price ea.]]*BOM[[#This Row],[Qty]]</f>
+        <v>3.39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4</v>
       </c>
@@ -1806,8 +2028,18 @@
       <c r="K13" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L13" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="M13">
+        <v>2E-3</v>
+      </c>
+      <c r="N13">
+        <f>BOM[[#This Row],[Price ea.]]*BOM[[#This Row],[Qty]]</f>
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1830,13 +2062,23 @@
         <v>80</v>
       </c>
       <c r="H14" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="K14" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="M14">
+        <v>1E-3</v>
+      </c>
+      <c r="N14">
+        <f>BOM[[#This Row],[Price ea.]]*BOM[[#This Row],[Qty]]</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1853,19 +2095,29 @@
         <v>45</v>
       </c>
       <c r="F15" t="s">
+        <v>118</v>
+      </c>
+      <c r="G15" t="s">
+        <v>119</v>
+      </c>
+      <c r="H15" t="s">
+        <v>121</v>
+      </c>
+      <c r="K15" t="s">
         <v>120</v>
       </c>
-      <c r="G15" t="s">
-        <v>121</v>
-      </c>
-      <c r="H15" t="s">
-        <v>123</v>
-      </c>
-      <c r="K15" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L15" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="M15">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="N15">
+        <f>BOM[[#This Row],[Price ea.]]*BOM[[#This Row],[Qty]]</f>
+        <v>8.7999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1882,19 +2134,29 @@
         <v>49</v>
       </c>
       <c r="F16" t="s">
+        <v>122</v>
+      </c>
+      <c r="G16" t="s">
+        <v>123</v>
+      </c>
+      <c r="H16" t="s">
+        <v>125</v>
+      </c>
+      <c r="K16" t="s">
         <v>124</v>
       </c>
-      <c r="G16" t="s">
-        <v>125</v>
-      </c>
-      <c r="H16" t="s">
-        <v>127</v>
-      </c>
-      <c r="K16" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L16" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="M16">
+        <v>0.69099999999999995</v>
+      </c>
+      <c r="N16">
+        <f>BOM[[#This Row],[Price ea.]]*BOM[[#This Row],[Qty]]</f>
+        <v>0.69099999999999995</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3</v>
       </c>
@@ -1917,13 +2179,23 @@
         <v>80</v>
       </c>
       <c r="H17" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="K17" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="M17">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="N17">
+        <f>BOM[[#This Row],[Price ea.]]*BOM[[#This Row],[Qty]]</f>
+        <v>0.20100000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2</v>
       </c>
@@ -1951,8 +2223,18 @@
       <c r="K18" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L18" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="M18">
+        <v>0.11</v>
+      </c>
+      <c r="N18">
+        <f>BOM[[#This Row],[Price ea.]]*BOM[[#This Row],[Qty]]</f>
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1</v>
       </c>
@@ -1980,8 +2262,18 @@
       <c r="K19" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L19" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="M19">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="N19">
+        <f>BOM[[#This Row],[Price ea.]]*BOM[[#This Row],[Qty]]</f>
+        <v>1.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>4</v>
       </c>
@@ -2004,13 +2296,23 @@
         <v>80</v>
       </c>
       <c r="H20" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="K20" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="M20">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="N20">
+        <f>BOM[[#This Row],[Price ea.]]*BOM[[#This Row],[Qty]]</f>
+        <v>0.26800000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1</v>
       </c>
@@ -2018,7 +2320,7 @@
         <v>55</v>
       </c>
       <c r="C21" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D21" t="s">
         <v>56</v>
@@ -2027,16 +2329,26 @@
         <v>57</v>
       </c>
       <c r="G21" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H21" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="I21" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="L21" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="M21">
+        <v>1.44</v>
+      </c>
+      <c r="N21">
+        <f>BOM[[#This Row],[Price ea.]]*BOM[[#This Row],[Qty]]</f>
+        <v>1.44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1</v>
       </c>
@@ -2044,28 +2356,38 @@
         <v>58</v>
       </c>
       <c r="C22" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D22" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E22" t="s">
         <v>59</v>
       </c>
       <c r="G22" t="s">
+        <v>126</v>
+      </c>
+      <c r="H22" t="s">
+        <v>127</v>
+      </c>
+      <c r="I22" t="s">
+        <v>135</v>
+      </c>
+      <c r="K22" t="s">
         <v>128</v>
       </c>
-      <c r="H22" t="s">
-        <v>129</v>
-      </c>
-      <c r="I22" t="s">
-        <v>137</v>
-      </c>
-      <c r="K22" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L22" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="M22">
+        <v>1.37</v>
+      </c>
+      <c r="N22">
+        <f>BOM[[#This Row],[Price ea.]]*BOM[[#This Row],[Qty]]</f>
+        <v>1.37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
@@ -2085,19 +2407,29 @@
         <v>64</v>
       </c>
       <c r="G23" t="s">
+        <v>136</v>
+      </c>
+      <c r="H23" t="s">
+        <v>139</v>
+      </c>
+      <c r="I23" t="s">
+        <v>137</v>
+      </c>
+      <c r="K23" t="s">
         <v>138</v>
       </c>
-      <c r="H23" t="s">
-        <v>141</v>
-      </c>
-      <c r="I23" t="s">
-        <v>139</v>
-      </c>
-      <c r="K23" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L23" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="M23">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="N23">
+        <f>BOM[[#This Row],[Price ea.]]*BOM[[#This Row],[Qty]]</f>
+        <v>9.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
@@ -2114,19 +2446,29 @@
         <v>67</v>
       </c>
       <c r="F24" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G24" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H24" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="I24" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="M24">
+        <v>7.87</v>
+      </c>
+      <c r="N24">
+        <f>BOM[[#This Row],[Price ea.]]*BOM[[#This Row],[Qty]]</f>
+        <v>7.87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1</v>
       </c>
@@ -2146,48 +2488,68 @@
         <v>71</v>
       </c>
       <c r="G25" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H25" t="s">
         <v>68</v>
       </c>
       <c r="I25" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="K25" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L25" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="M25">
+        <v>4.72</v>
+      </c>
+      <c r="N25">
+        <f>BOM[[#This Row],[Price ea.]]*BOM[[#This Row],[Qty]]</f>
+        <v>4.72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1</v>
       </c>
       <c r="B26" t="s">
+        <v>149</v>
+      </c>
+      <c r="C26" t="s">
+        <v>150</v>
+      </c>
+      <c r="D26" t="s">
+        <v>151</v>
+      </c>
+      <c r="E26" t="s">
+        <v>152</v>
+      </c>
+      <c r="F26" t="s">
+        <v>153</v>
+      </c>
+      <c r="G26" t="s">
         <v>154</v>
       </c>
-      <c r="C26" t="s">
+      <c r="H26" t="s">
         <v>155</v>
       </c>
-      <c r="D26" t="s">
-        <v>156</v>
-      </c>
-      <c r="E26" t="s">
-        <v>157</v>
-      </c>
-      <c r="F26" t="s">
-        <v>158</v>
-      </c>
-      <c r="G26" t="s">
-        <v>159</v>
-      </c>
-      <c r="H26" t="s">
-        <v>160</v>
-      </c>
       <c r="J26" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="M26">
+        <v>2.75</v>
+      </c>
+      <c r="N26">
+        <f>BOM[[#This Row],[Price ea.]]*BOM[[#This Row],[Qty]]</f>
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1</v>
       </c>
@@ -2201,34 +2563,75 @@
         <v>73</v>
       </c>
       <c r="E27" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="F27" t="s">
         <v>74</v>
       </c>
       <c r="G27" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="H27" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="K27" t="s">
-        <v>150</v>
-      </c>
-      <c r="L27" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>153</v>
+        <v>146</v>
+      </c>
+      <c r="L27" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="M27" s="1">
+        <v>0.69599999999999995</v>
+      </c>
+      <c r="N27">
+        <f>BOM[[#This Row],[Price ea.]]*BOM[[#This Row],[Qty]]</f>
+        <v>0.69599999999999995</v>
+      </c>
+      <c r="O27" s="1"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="M29" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="N29" s="5">
+        <f>SUM(BOM[Price ea. Order])</f>
+        <v>25.251000000000001</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="L7" r:id="rId1"/>
+    <hyperlink ref="L6" r:id="rId2"/>
+    <hyperlink ref="L5" r:id="rId3"/>
+    <hyperlink ref="L4" r:id="rId4"/>
+    <hyperlink ref="L3" r:id="rId5"/>
+    <hyperlink ref="L2" r:id="rId6"/>
+    <hyperlink ref="L8" r:id="rId7"/>
+    <hyperlink ref="L9" r:id="rId8"/>
+    <hyperlink ref="L10" r:id="rId9"/>
+    <hyperlink ref="L11" r:id="rId10"/>
+    <hyperlink ref="L12" r:id="rId11"/>
+    <hyperlink ref="L13" r:id="rId12"/>
+    <hyperlink ref="L14" r:id="rId13"/>
+    <hyperlink ref="L15" r:id="rId14"/>
+    <hyperlink ref="L16" r:id="rId15"/>
+    <hyperlink ref="L17" r:id="rId16"/>
+    <hyperlink ref="L18" r:id="rId17"/>
+    <hyperlink ref="L19" r:id="rId18"/>
+    <hyperlink ref="L20" r:id="rId19"/>
+    <hyperlink ref="L21" r:id="rId20"/>
+    <hyperlink ref="L22" r:id="rId21"/>
+    <hyperlink ref="L23" r:id="rId22"/>
+    <hyperlink ref="L24" r:id="rId23"/>
+    <hyperlink ref="L25" r:id="rId24"/>
+    <hyperlink ref="L26" r:id="rId25"/>
+    <hyperlink ref="L27" r:id="rId26"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId27"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId28"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated BOM to include R17 - a minor oversight in the original BOM
</commit_message>
<xml_diff>
--- a/Hardware/bom_r2.xlsx
+++ b/Hardware/bom_r2.xlsx
@@ -97,9 +97,6 @@
     <t>R0603</t>
   </si>
   <si>
-    <t>R1, R4</t>
-  </si>
-  <si>
     <t>12.4K</t>
   </si>
   <si>
@@ -629,6 +626,9 @@
   </si>
   <si>
     <t>Final Order Cost:</t>
+  </si>
+  <si>
+    <t>R1, R4, R17</t>
   </si>
 </sst>
 </file>
@@ -1520,8 +1520,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O32" sqref="O32"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1567,25 +1567,25 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L1" t="s">
+        <v>169</v>
+      </c>
+      <c r="M1" t="s">
         <v>170</v>
       </c>
-      <c r="M1" t="s">
-        <v>171</v>
-      </c>
       <c r="N1" t="s">
+        <v>200</v>
+      </c>
+      <c r="O1" t="s">
         <v>201</v>
-      </c>
-      <c r="O1" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -1593,7 +1593,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -1602,22 +1602,22 @@
         <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M2">
         <v>0.248</v>
@@ -1648,19 +1648,19 @@
         <v>14</v>
       </c>
       <c r="F3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G3" t="s">
         <v>90</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
+        <v>92</v>
+      </c>
+      <c r="K3" t="s">
         <v>91</v>
       </c>
-      <c r="H3" t="s">
-        <v>93</v>
-      </c>
-      <c r="K3" t="s">
-        <v>92</v>
-      </c>
       <c r="L3" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M3">
         <v>2E-3</v>
@@ -1691,19 +1691,19 @@
         <v>18</v>
       </c>
       <c r="F4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G4" t="s">
         <v>90</v>
       </c>
-      <c r="G4" t="s">
-        <v>91</v>
-      </c>
       <c r="H4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="M4">
         <v>0.16200000000000001</v>
@@ -1722,7 +1722,7 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C5" t="s">
         <v>19</v>
@@ -1731,22 +1731,22 @@
         <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F5" t="s">
+        <v>89</v>
+      </c>
+      <c r="G5" t="s">
         <v>90</v>
       </c>
-      <c r="G5" t="s">
-        <v>91</v>
-      </c>
       <c r="H5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M5">
         <v>6.0000000000000001E-3</v>
@@ -1765,7 +1765,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C6" t="s">
         <v>19</v>
@@ -1774,22 +1774,22 @@
         <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F6" t="s">
+        <v>89</v>
+      </c>
+      <c r="G6" t="s">
         <v>90</v>
       </c>
-      <c r="G6" t="s">
-        <v>91</v>
-      </c>
       <c r="H6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M6">
         <v>0.24</v>
@@ -1808,7 +1808,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C7" t="s">
         <v>21</v>
@@ -1820,19 +1820,19 @@
         <v>23</v>
       </c>
       <c r="F7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M7">
         <v>2E-3</v>
@@ -1860,22 +1860,22 @@
         <v>26</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>204</v>
       </c>
       <c r="F8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H8" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="L8" s="3" t="s">
         <v>179</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>180</v>
       </c>
       <c r="M8">
         <v>1.6E-2</v>
@@ -1894,7 +1894,7 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
         <v>25</v>
@@ -1903,22 +1903,22 @@
         <v>26</v>
       </c>
       <c r="E9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M9">
         <v>1E-3</v>
@@ -1937,34 +1937,34 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D10" t="s">
         <v>26</v>
       </c>
       <c r="E10" t="s">
+        <v>158</v>
+      </c>
+      <c r="F10" t="s">
+        <v>99</v>
+      </c>
+      <c r="G10" t="s">
+        <v>161</v>
+      </c>
+      <c r="H10" t="s">
+        <v>163</v>
+      </c>
+      <c r="I10" t="s">
+        <v>160</v>
+      </c>
+      <c r="K10" t="s">
         <v>159</v>
       </c>
-      <c r="F10" t="s">
-        <v>100</v>
-      </c>
-      <c r="G10" t="s">
-        <v>162</v>
-      </c>
-      <c r="H10" t="s">
-        <v>164</v>
-      </c>
-      <c r="I10" t="s">
-        <v>161</v>
-      </c>
-      <c r="K10" t="s">
-        <v>160</v>
-      </c>
       <c r="L10" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M10">
         <v>0.1</v>
@@ -1983,7 +1983,7 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
         <v>25</v>
@@ -1992,22 +1992,22 @@
         <v>26</v>
       </c>
       <c r="E11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="M11">
         <v>6.7000000000000004E-2</v>
@@ -2026,31 +2026,31 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
         <v>32</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>33</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
+        <v>155</v>
+      </c>
+      <c r="F12" t="s">
         <v>34</v>
       </c>
-      <c r="E12" t="s">
-        <v>156</v>
-      </c>
-      <c r="F12" t="s">
-        <v>35</v>
-      </c>
       <c r="G12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H12" t="s">
+        <v>75</v>
+      </c>
+      <c r="K12" t="s">
         <v>76</v>
       </c>
-      <c r="K12" t="s">
-        <v>77</v>
-      </c>
       <c r="L12" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="M12">
         <v>3.39</v>
@@ -2069,31 +2069,31 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="s">
         <v>36</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>37</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>38</v>
       </c>
-      <c r="E13" t="s">
-        <v>39</v>
-      </c>
       <c r="F13" t="s">
+        <v>89</v>
+      </c>
+      <c r="G13" t="s">
         <v>90</v>
       </c>
-      <c r="G13" t="s">
-        <v>91</v>
-      </c>
       <c r="H13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M13">
         <v>2E-3</v>
@@ -2112,7 +2112,7 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
         <v>21</v>
@@ -2121,22 +2121,22 @@
         <v>22</v>
       </c>
       <c r="E14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="M14">
         <v>1E-3</v>
@@ -2155,31 +2155,31 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
         <v>42</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>43</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>44</v>
       </c>
-      <c r="E15" t="s">
-        <v>45</v>
-      </c>
       <c r="F15" t="s">
+        <v>117</v>
+      </c>
+      <c r="G15" t="s">
         <v>118</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
+        <v>120</v>
+      </c>
+      <c r="K15" t="s">
         <v>119</v>
       </c>
-      <c r="H15" t="s">
-        <v>121</v>
-      </c>
-      <c r="K15" t="s">
-        <v>120</v>
-      </c>
       <c r="L15" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="M15">
         <v>4.3999999999999997E-2</v>
@@ -2198,31 +2198,31 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" t="s">
         <v>46</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>47</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>48</v>
       </c>
-      <c r="E16" t="s">
-        <v>49</v>
-      </c>
       <c r="F16" t="s">
+        <v>121</v>
+      </c>
+      <c r="G16" t="s">
         <v>122</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
+        <v>124</v>
+      </c>
+      <c r="K16" t="s">
         <v>123</v>
       </c>
-      <c r="H16" t="s">
-        <v>125</v>
-      </c>
-      <c r="K16" t="s">
-        <v>124</v>
-      </c>
       <c r="L16" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="M16">
         <v>0.69099999999999995</v>
@@ -2241,7 +2241,7 @@
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C17" t="s">
         <v>21</v>
@@ -2250,22 +2250,22 @@
         <v>22</v>
       </c>
       <c r="E17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="M17">
         <v>6.7000000000000004E-2</v>
@@ -2284,31 +2284,31 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" t="s">
         <v>51</v>
       </c>
-      <c r="C18" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" t="s">
-        <v>38</v>
-      </c>
-      <c r="E18" t="s">
-        <v>52</v>
-      </c>
       <c r="F18" t="s">
+        <v>89</v>
+      </c>
+      <c r="G18" t="s">
         <v>90</v>
       </c>
-      <c r="G18" t="s">
-        <v>91</v>
-      </c>
       <c r="H18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="M18">
         <v>0.11</v>
@@ -2327,7 +2327,7 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C19" t="s">
         <v>12</v>
@@ -2336,22 +2336,22 @@
         <v>13</v>
       </c>
       <c r="E19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F19" t="s">
+        <v>89</v>
+      </c>
+      <c r="G19" t="s">
         <v>90</v>
       </c>
-      <c r="G19" t="s">
-        <v>91</v>
-      </c>
       <c r="H19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="M19">
         <v>1.2999999999999999E-2</v>
@@ -2370,7 +2370,7 @@
         <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C20" t="s">
         <v>21</v>
@@ -2379,22 +2379,22 @@
         <v>22</v>
       </c>
       <c r="E20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="M20">
         <v>6.7000000000000004E-2</v>
@@ -2413,28 +2413,28 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" t="s">
+        <v>130</v>
+      </c>
+      <c r="D21" t="s">
         <v>55</v>
       </c>
-      <c r="C21" t="s">
-        <v>131</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>56</v>
       </c>
-      <c r="E21" t="s">
-        <v>57</v>
-      </c>
       <c r="G21" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H21" t="s">
+        <v>132</v>
+      </c>
+      <c r="I21" t="s">
         <v>133</v>
       </c>
-      <c r="I21" t="s">
-        <v>134</v>
-      </c>
       <c r="L21" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="M21">
         <v>1.44</v>
@@ -2453,31 +2453,31 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" t="s">
+        <v>129</v>
+      </c>
+      <c r="D22" t="s">
+        <v>126</v>
+      </c>
+      <c r="E22" t="s">
         <v>58</v>
       </c>
-      <c r="C22" t="s">
-        <v>130</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="G22" t="s">
+        <v>125</v>
+      </c>
+      <c r="H22" t="s">
+        <v>126</v>
+      </c>
+      <c r="I22" t="s">
+        <v>134</v>
+      </c>
+      <c r="K22" t="s">
         <v>127</v>
       </c>
-      <c r="E22" t="s">
-        <v>59</v>
-      </c>
-      <c r="G22" t="s">
-        <v>126</v>
-      </c>
-      <c r="H22" t="s">
-        <v>127</v>
-      </c>
-      <c r="I22" t="s">
-        <v>135</v>
-      </c>
-      <c r="K22" t="s">
-        <v>128</v>
-      </c>
       <c r="L22" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="M22">
         <v>1.37</v>
@@ -2496,34 +2496,34 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" t="s">
         <v>60</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>61</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>62</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>63</v>
       </c>
-      <c r="F23" t="s">
-        <v>64</v>
-      </c>
       <c r="G23" t="s">
+        <v>135</v>
+      </c>
+      <c r="H23" t="s">
+        <v>138</v>
+      </c>
+      <c r="I23" t="s">
         <v>136</v>
       </c>
-      <c r="H23" t="s">
-        <v>139</v>
-      </c>
-      <c r="I23" t="s">
+      <c r="K23" t="s">
         <v>137</v>
       </c>
-      <c r="K23" t="s">
-        <v>138</v>
-      </c>
       <c r="L23" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="M23">
         <v>9.2999999999999999E-2</v>
@@ -2542,31 +2542,31 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" t="s">
         <v>65</v>
       </c>
-      <c r="C24" t="s">
-        <v>65</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>66</v>
       </c>
-      <c r="E24" t="s">
-        <v>67</v>
-      </c>
       <c r="F24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G24" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H24" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="M24">
         <v>7.87</v>
@@ -2585,34 +2585,34 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" t="s">
+        <v>67</v>
+      </c>
+      <c r="D25" t="s">
         <v>68</v>
       </c>
-      <c r="C25" t="s">
-        <v>68</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>69</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>70</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
+        <v>141</v>
+      </c>
+      <c r="H25" t="s">
+        <v>67</v>
+      </c>
+      <c r="I25" t="s">
+        <v>144</v>
+      </c>
+      <c r="K25" t="s">
         <v>71</v>
       </c>
-      <c r="G25" t="s">
-        <v>142</v>
-      </c>
-      <c r="H25" t="s">
-        <v>68</v>
-      </c>
-      <c r="I25" t="s">
-        <v>145</v>
-      </c>
-      <c r="K25" t="s">
-        <v>72</v>
-      </c>
       <c r="L25" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="M25">
         <v>4.72</v>
@@ -2631,31 +2631,31 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
+        <v>148</v>
+      </c>
+      <c r="C26" t="s">
         <v>149</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>150</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>151</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>152</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>153</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>154</v>
       </c>
-      <c r="H26" t="s">
-        <v>155</v>
-      </c>
       <c r="J26" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="M26">
         <v>2.75</v>
@@ -2674,31 +2674,31 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" t="s">
+        <v>72</v>
+      </c>
+      <c r="D27" t="s">
+        <v>72</v>
+      </c>
+      <c r="E27" t="s">
+        <v>165</v>
+      </c>
+      <c r="F27" t="s">
         <v>73</v>
       </c>
-      <c r="C27" t="s">
-        <v>73</v>
-      </c>
-      <c r="D27" t="s">
-        <v>73</v>
-      </c>
-      <c r="E27" t="s">
-        <v>166</v>
-      </c>
-      <c r="F27" t="s">
-        <v>74</v>
-      </c>
       <c r="G27" t="s">
+        <v>146</v>
+      </c>
+      <c r="H27" t="s">
         <v>147</v>
       </c>
-      <c r="H27" t="s">
-        <v>148</v>
-      </c>
       <c r="K27" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M27" s="1">
         <v>0.69599999999999995</v>
@@ -2716,7 +2716,7 @@
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="M29" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="N29" s="5">
         <f>SUM(BOM[Price ea. Order])</f>
@@ -2725,7 +2725,7 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="M30" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="N30" s="5">
         <v>50</v>
@@ -2733,7 +2733,7 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="M31" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="N31" s="5">
         <f>N29*N30</f>

</xml_diff>

<commit_message>
fixed BOM issue with 56kOhm vs. 56 ohm resistor (R15)
</commit_message>
<xml_diff>
--- a/Hardware/bom_r2.xlsx
+++ b/Hardware/bom_r2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="203">
   <si>
     <t>Qty</t>
   </si>
@@ -493,21 +493,9 @@
     <t>R15</t>
   </si>
   <si>
-    <t>05R3863</t>
-  </si>
-  <si>
-    <t>1276-4545-1-ND</t>
-  </si>
-  <si>
-    <t>Samsung NA</t>
-  </si>
-  <si>
     <t>56K</t>
   </si>
   <si>
-    <t>RC1608F560CS</t>
-  </si>
-  <si>
     <t>C1, C2, C3, C4, C5, C6, C7, C8, C9, C10, C11, C12, C14, C15, C16</t>
   </si>
   <si>
@@ -559,9 +547,6 @@
     <t>http://www.newark.com/multicomp/mc0063w0603112k4/resistor-12k4-0-063w-1-0603/dp/94W4696?ost=94W4696</t>
   </si>
   <si>
-    <t>http://www.digikey.com/product-search/en?x=0&amp;y=0&amp;lang=en&amp;site=us&amp;keywords=1276-4545-1-ND</t>
-  </si>
-  <si>
     <t>http://www.newark.com/multicomp/mc0603saf1202t5e/thick-film-resistor-12kohm-100mw/dp/79M5909?ost=79M5909</t>
   </si>
   <si>
@@ -629,6 +614,15 @@
   </si>
   <si>
     <t>R1, R4, R17</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/panasonic-electronic-components/erj-p03f5602v/thick-film-resistor-56kohm-1-0603/dp/05X8647</t>
+  </si>
+  <si>
+    <t>05X8647</t>
+  </si>
+  <si>
+    <t> ERJ-P03F5602V</t>
   </si>
 </sst>
 </file>
@@ -1520,8 +1514,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1570,22 +1564,22 @@
         <v>131</v>
       </c>
       <c r="J1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="K1" t="s">
         <v>74</v>
       </c>
       <c r="L1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="M1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="N1" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="O1" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -1602,7 +1596,7 @@
         <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -1617,7 +1611,7 @@
         <v>80</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="M2">
         <v>0.248</v>
@@ -1628,7 +1622,7 @@
       </c>
       <c r="O2">
         <f>N30*BOM[[#This Row],[Qty]]</f>
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -1660,7 +1654,7 @@
         <v>91</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="M3">
         <v>2E-3</v>
@@ -1671,7 +1665,7 @@
       </c>
       <c r="O3">
         <f>N30*BOM[[#This Row],[Qty]]</f>
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -1703,7 +1697,7 @@
         <v>93</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="M4">
         <v>0.16200000000000001</v>
@@ -1714,7 +1708,7 @@
       </c>
       <c r="O4">
         <f>N30*BOM[[#This Row],[Qty]]</f>
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -1731,7 +1725,7 @@
         <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F5" t="s">
         <v>89</v>
@@ -1746,7 +1740,7 @@
         <v>95</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="M5">
         <v>6.0000000000000001E-3</v>
@@ -1757,7 +1751,7 @@
       </c>
       <c r="O5">
         <f>N30*BOM[[#This Row],[Qty]]</f>
-        <v>750</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -1789,7 +1783,7 @@
         <v>97</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="M6">
         <v>0.24</v>
@@ -1800,7 +1794,7 @@
       </c>
       <c r="O6">
         <f>N30*BOM[[#This Row],[Qty]]</f>
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -1832,7 +1826,7 @@
         <v>106</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="M7">
         <v>2E-3</v>
@@ -1843,7 +1837,7 @@
       </c>
       <c r="O7">
         <f>N30*BOM[[#This Row],[Qty]]</f>
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -1860,7 +1854,7 @@
         <v>26</v>
       </c>
       <c r="E8" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="F8" t="s">
         <v>99</v>
@@ -1869,13 +1863,13 @@
         <v>79</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="M8">
         <v>1.6E-2</v>
@@ -1886,7 +1880,7 @@
       </c>
       <c r="O8">
         <f>N30*BOM[[#This Row],[Qty]]</f>
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -1918,7 +1912,7 @@
         <v>108</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="M9">
         <v>1E-3</v>
@@ -1929,7 +1923,7 @@
       </c>
       <c r="O9">
         <f>N30*BOM[[#This Row],[Qty]]</f>
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -1937,7 +1931,7 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C10" t="s">
         <v>157</v>
@@ -1952,30 +1946,27 @@
         <v>99</v>
       </c>
       <c r="G10" t="s">
-        <v>161</v>
-      </c>
-      <c r="H10" t="s">
-        <v>163</v>
-      </c>
-      <c r="I10" t="s">
-        <v>160</v>
-      </c>
-      <c r="K10" t="s">
-        <v>159</v>
+        <v>77</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>201</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>181</v>
+        <v>200</v>
       </c>
       <c r="M10">
-        <v>0.1</v>
+        <v>3.1E-2</v>
       </c>
       <c r="N10">
         <f>BOM[[#This Row],[Price ea.]]*BOM[[#This Row],[Qty]]</f>
-        <v>0.1</v>
+        <v>3.1E-2</v>
       </c>
       <c r="O10">
         <f>N30*BOM[[#This Row],[Qty]]</f>
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -2007,7 +1998,7 @@
         <v>110</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="M11">
         <v>6.7000000000000004E-2</v>
@@ -2018,7 +2009,7 @@
       </c>
       <c r="O11">
         <f>N30*BOM[[#This Row],[Qty]]</f>
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -2050,7 +2041,7 @@
         <v>76</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="M12">
         <v>3.39</v>
@@ -2061,7 +2052,7 @@
       </c>
       <c r="O12">
         <f>N30*BOM[[#This Row],[Qty]]</f>
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -2093,7 +2084,7 @@
         <v>100</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="M13">
         <v>2E-3</v>
@@ -2104,7 +2095,7 @@
       </c>
       <c r="O13">
         <f>N30*BOM[[#This Row],[Qty]]</f>
-        <v>200</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -2136,7 +2127,7 @@
         <v>112</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="M14">
         <v>1E-3</v>
@@ -2147,7 +2138,7 @@
       </c>
       <c r="O14">
         <f>N30*BOM[[#This Row],[Qty]]</f>
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -2179,7 +2170,7 @@
         <v>119</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="M15">
         <v>4.3999999999999997E-2</v>
@@ -2190,7 +2181,7 @@
       </c>
       <c r="O15">
         <f>N30*BOM[[#This Row],[Qty]]</f>
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -2222,7 +2213,7 @@
         <v>123</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="M16">
         <v>0.69099999999999995</v>
@@ -2233,7 +2224,7 @@
       </c>
       <c r="O16">
         <f>N30*BOM[[#This Row],[Qty]]</f>
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
@@ -2265,7 +2256,7 @@
         <v>128</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="M17">
         <v>6.7000000000000004E-2</v>
@@ -2276,7 +2267,7 @@
       </c>
       <c r="O17">
         <f>N30*BOM[[#This Row],[Qty]]</f>
-        <v>150</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
@@ -2308,7 +2299,7 @@
         <v>102</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="M18">
         <v>0.11</v>
@@ -2319,7 +2310,7 @@
       </c>
       <c r="O18">
         <f>N30*BOM[[#This Row],[Qty]]</f>
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
@@ -2351,7 +2342,7 @@
         <v>104</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="M19">
         <v>1.2999999999999999E-2</v>
@@ -2362,7 +2353,7 @@
       </c>
       <c r="O19">
         <f>N30*BOM[[#This Row],[Qty]]</f>
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
@@ -2394,7 +2385,7 @@
         <v>115</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="M20">
         <v>6.7000000000000004E-2</v>
@@ -2405,7 +2396,7 @@
       </c>
       <c r="O20">
         <f>N30*BOM[[#This Row],[Qty]]</f>
-        <v>200</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
@@ -2434,7 +2425,7 @@
         <v>133</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="M21">
         <v>1.44</v>
@@ -2445,7 +2436,7 @@
       </c>
       <c r="O21">
         <f>N30*BOM[[#This Row],[Qty]]</f>
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -2477,7 +2468,7 @@
         <v>127</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="M22">
         <v>1.37</v>
@@ -2488,7 +2479,7 @@
       </c>
       <c r="O22">
         <f>N30*BOM[[#This Row],[Qty]]</f>
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
@@ -2523,7 +2514,7 @@
         <v>137</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="M23">
         <v>9.2999999999999999E-2</v>
@@ -2534,7 +2525,7 @@
       </c>
       <c r="O23">
         <f>N30*BOM[[#This Row],[Qty]]</f>
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
@@ -2566,7 +2557,7 @@
         <v>139</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="M24">
         <v>7.87</v>
@@ -2577,7 +2568,7 @@
       </c>
       <c r="O24">
         <f>N30*BOM[[#This Row],[Qty]]</f>
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
@@ -2612,7 +2603,7 @@
         <v>71</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="M25">
         <v>4.72</v>
@@ -2623,7 +2614,7 @@
       </c>
       <c r="O25">
         <f>N30*BOM[[#This Row],[Qty]]</f>
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
@@ -2652,10 +2643,10 @@
         <v>154</v>
       </c>
       <c r="J26" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="M26">
         <v>2.75</v>
@@ -2666,7 +2657,7 @@
       </c>
       <c r="O26">
         <f>N30*BOM[[#This Row],[Qty]]</f>
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
@@ -2683,7 +2674,7 @@
         <v>72</v>
       </c>
       <c r="E27" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="F27" t="s">
         <v>73</v>
@@ -2698,7 +2689,7 @@
         <v>145</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="M27" s="1">
         <v>0.69599999999999995</v>
@@ -2709,35 +2700,35 @@
       </c>
       <c r="O27">
         <f>N30*BOM[[#This Row],[Qty]]</f>
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="P27" s="1"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="M29" s="5" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="N29" s="5">
         <f>SUM(BOM[Price ea. Order])</f>
-        <v>25.251000000000001</v>
+        <v>25.182000000000002</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="M30" s="5" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="N30" s="5">
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="M31" s="6" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="N31" s="5">
         <f>N29*N30</f>
-        <v>1262.55</v>
+        <v>125.91000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>